<commit_message>
Post survey graphs and likert data
</commit_message>
<xml_diff>
--- a/Data/GGEE_23_EndofCamp_Likert.xlsx
+++ b/Data/GGEE_23_EndofCamp_Likert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviarandell/Documents/GitHub/GGEESummer23/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31B4734-A6F4-C74F-9DAD-B8FCC18030C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{517103B1-6333-5542-9D06-67E637CAFCC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15420" yWindow="500" windowWidth="13380" windowHeight="15760" firstSheet="3" activeTab="5" xr2:uid="{7292BB22-2922-0840-9871-47BBFB9FAADB}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="19">
   <si>
     <t>A lot of experience</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">Basic </t>
+  </si>
+  <si>
+    <t>How would you rate your coding skills before the summer program?</t>
+  </si>
+  <si>
+    <t>How would you rate your coding skills after the summer program?</t>
   </si>
 </sst>
 </file>
@@ -2068,7 +2074,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2095,7 +2101,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B2" s="4">
         <v>6.5693430700000004</v>
@@ -2874,7 +2880,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2901,7 +2907,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B2" s="5">
         <v>29.197080291970799</v>

</xml_diff>